<commit_message>
updated projects for dir name change
</commit_message>
<xml_diff>
--- a/projects/SEB_calibration_NSGA_2013.xlsx
+++ b/projects/SEB_calibration_NSGA_2013.xlsx
@@ -2428,21 +2428,6 @@
     <t>0.4.2</t>
   </si>
   <si>
-    <t>bball</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/lib</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/seeds/SEB4_baseboard.osm</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/weather/SRRL_2013AMY_60min.epw</t>
-  </si>
-  <si>
-    <t>../ASHRAE_example/measures</t>
-  </si>
-  <si>
     <t>Parameter Short Display Name</t>
   </si>
   <si>
@@ -2462,6 +2447,21 @@
   </si>
   <si>
     <t>default</t>
+  </si>
+  <si>
+    <t>../Calibration_example/measures</t>
+  </si>
+  <si>
+    <t>../Calibration_example/weather/SRRL_2013AMY_60min.epw</t>
+  </si>
+  <si>
+    <t>../Calibration_example/seeds/SEB4_baseboard.osm</t>
+  </si>
+  <si>
+    <t>../Calibration_example/lib</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -6798,7 +6798,7 @@
   <dimension ref="A1:E44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6845,7 +6845,7 @@
         <v>456</v>
       </c>
       <c r="B4" s="25" t="s">
-        <v>795</v>
+        <v>806</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>457</v>
@@ -6856,7 +6856,7 @@
         <v>469</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>805</v>
+        <v>800</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>614</v>
@@ -6867,7 +6867,7 @@
         <v>470</v>
       </c>
       <c r="B6" s="25" t="s">
-        <v>806</v>
+        <v>801</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>472</v>
@@ -6949,7 +6949,7 @@
         <v>25</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>799</v>
+        <v>802</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>654</v>
@@ -7191,7 +7191,7 @@
         <v>29</v>
       </c>
       <c r="B37" s="25" t="s">
-        <v>798</v>
+        <v>803</v>
       </c>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7219,7 +7219,7 @@
         <v>643</v>
       </c>
       <c r="D40" s="31" t="s">
-        <v>797</v>
+        <v>804</v>
       </c>
       <c r="E40" s="2"/>
     </row>
@@ -7246,7 +7246,7 @@
         <v>645</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>796</v>
+        <v>805</v>
       </c>
     </row>
     <row r="44" spans="1:5" s="31" customFormat="1" x14ac:dyDescent="0.3">
@@ -7379,7 +7379,7 @@
         <v>36</v>
       </c>
       <c r="F3" s="63" t="s">
-        <v>800</v>
+        <v>795</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -10060,7 +10060,7 @@
         <v>459</v>
       </c>
       <c r="B2" s="66" t="s">
-        <v>801</v>
+        <v>796</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>632</v>
@@ -10098,7 +10098,7 @@
         <v>624</v>
       </c>
       <c r="B3" s="66" t="s">
-        <v>802</v>
+        <v>797</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>637</v>
@@ -10196,7 +10196,7 @@
         <v>641</v>
       </c>
       <c r="B6" s="48" t="s">
-        <v>803</v>
+        <v>798</v>
       </c>
       <c r="C6" s="30" t="s">
         <v>636</v>
@@ -10228,7 +10228,7 @@
         <v>642</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>804</v>
+        <v>799</v>
       </c>
       <c r="C7" s="30" t="s">
         <v>635</v>

</xml_diff>

<commit_message>
update examples to test Server 2.0
</commit_message>
<xml_diff>
--- a/projects/SEB_calibration_NSGA_2013.xlsx
+++ b/projects/SEB_calibration_NSGA_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="1"/>
+    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2445,45 +2445,6 @@
     <t>set_runperiod</t>
   </si>
   <si>
-    <t>CalibrationReportsEnhanced</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.electric_bill_nmbe_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced.gas_bill_nmbe_within_limit</t>
-  </si>
-  <si>
     <t>default</t>
   </si>
   <si>
@@ -2494,6 +2455,45 @@
   </si>
   <si>
     <t>1.21.14</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_modeled</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_rmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.electricity_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>calibration_reports_enhanced20.gas_nmbe_within_limit</t>
   </si>
 </sst>
 </file>
@@ -6848,7 +6848,7 @@
         <v>465</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>817</v>
+        <v>804</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>609</v>
@@ -6859,7 +6859,7 @@
         <v>466</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>814</v>
+        <v>801</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>468</v>
@@ -7246,9 +7246,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z200"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A76" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A103" sqref="A103:XFD103"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7772,13 +7772,13 @@
         <v>1</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>815</v>
+        <v>802</v>
       </c>
       <c r="C23" s="36" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="D23" s="36" t="s">
-        <v>801</v>
+        <v>805</v>
       </c>
       <c r="E23" s="36" t="s">
         <v>231</v>
@@ -7859,7 +7859,7 @@
         <v>1</v>
       </c>
       <c r="R26" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7914,7 +7914,7 @@
         <v>0.01</v>
       </c>
       <c r="R28" s="55" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -8091,7 +8091,7 @@
       </c>
       <c r="Q36" s="54"/>
       <c r="R36" s="51" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -8359,7 +8359,7 @@
         <v>1</v>
       </c>
       <c r="R46" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8582,7 +8582,7 @@
         <v>1</v>
       </c>
       <c r="R56" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -8823,7 +8823,7 @@
         <v>0.25</v>
       </c>
       <c r="R67" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9064,7 +9064,7 @@
         <v>1</v>
       </c>
       <c r="R78" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="79" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9105,7 +9105,7 @@
         <v>1</v>
       </c>
       <c r="R79" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9325,7 +9325,7 @@
         <v>1</v>
       </c>
       <c r="R89" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="90" spans="1:20" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9366,7 +9366,7 @@
         <v>1</v>
       </c>
       <c r="R90" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
@@ -9462,7 +9462,7 @@
       <c r="P93" s="39"/>
       <c r="Q93" s="39"/>
       <c r="R93" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="94" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9504,7 +9504,7 @@
       <c r="P94" s="39"/>
       <c r="Q94" s="39"/>
       <c r="R94" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9546,7 +9546,7 @@
       <c r="P95" s="41"/>
       <c r="Q95" s="41"/>
       <c r="R95" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
       <c r="T95" s="30"/>
     </row>
@@ -9620,7 +9620,7 @@
       <c r="P97" s="39"/>
       <c r="Q97" s="39"/>
       <c r="R97" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9662,7 +9662,7 @@
       <c r="P98" s="39"/>
       <c r="Q98" s="39"/>
       <c r="R98" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -9704,7 +9704,7 @@
       <c r="P99" s="41"/>
       <c r="Q99" s="41"/>
       <c r="R99" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="100" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -9762,7 +9762,7 @@
         <v>0.1</v>
       </c>
       <c r="R101" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="102" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9803,7 +9803,7 @@
         <v>50</v>
       </c>
       <c r="R102" s="39" t="s">
-        <v>816</v>
+        <v>803</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
@@ -10242,9 +10242,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26:XFD37"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11003,7 +11003,7 @@
       <c r="B26" s="46"/>
       <c r="C26" s="29"/>
       <c r="D26" s="29" t="s">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="E26" s="29" t="s">
         <v>643</v>
@@ -11032,7 +11032,7 @@
       <c r="B27" s="46"/>
       <c r="C27" s="29"/>
       <c r="D27" s="29" t="s">
-        <v>803</v>
+        <v>807</v>
       </c>
       <c r="E27" s="29" t="s">
         <v>645</v>
@@ -11061,7 +11061,7 @@
       <c r="B28" s="46"/>
       <c r="C28" s="29"/>
       <c r="D28" s="29" t="s">
-        <v>804</v>
+        <v>808</v>
       </c>
       <c r="E28" s="29" t="s">
         <v>651</v>
@@ -11089,7 +11089,7 @@
       <c r="B29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="29" t="s">
-        <v>805</v>
+        <v>809</v>
       </c>
       <c r="E29" s="29" t="s">
         <v>651</v>
@@ -11117,7 +11117,7 @@
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="29" t="s">
-        <v>806</v>
+        <v>810</v>
       </c>
       <c r="E30" s="29" t="s">
         <v>651</v>
@@ -11145,7 +11145,7 @@
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="29" t="s">
-        <v>807</v>
+        <v>811</v>
       </c>
       <c r="E31" s="29" t="s">
         <v>651</v>
@@ -11173,7 +11173,7 @@
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="29" t="s">
-        <v>808</v>
+        <v>812</v>
       </c>
       <c r="E32" s="29" t="s">
         <v>651</v>
@@ -11201,7 +11201,7 @@
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="29" t="s">
-        <v>809</v>
+        <v>813</v>
       </c>
       <c r="E33" s="29" t="s">
         <v>651</v>
@@ -11229,7 +11229,7 @@
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="29" t="s">
-        <v>810</v>
+        <v>814</v>
       </c>
       <c r="E34" s="29"/>
       <c r="F34" s="30" t="s">
@@ -11252,7 +11252,7 @@
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>
       <c r="D35" s="29" t="s">
-        <v>811</v>
+        <v>815</v>
       </c>
       <c r="E35" s="29"/>
       <c r="F35" s="30" t="s">
@@ -11275,7 +11275,7 @@
       <c r="B36" s="29"/>
       <c r="C36" s="29"/>
       <c r="D36" s="29" t="s">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="E36" s="29"/>
       <c r="F36" s="30" t="s">
@@ -11297,7 +11297,7 @@
       </c>
       <c r="B37" s="29"/>
       <c r="D37" s="29" t="s">
-        <v>813</v>
+        <v>817</v>
       </c>
       <c r="F37" s="30" t="s">
         <v>62</v>

</xml_diff>

<commit_message>
removing extra outputs to make debugging easier
</commit_message>
<xml_diff>
--- a/projects/SEB_calibration_NSGA_2013.xlsx
+++ b/projects/SEB_calibration_NSGA_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2656" uniqueCount="818">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2567" uniqueCount="769">
   <si>
     <t>type</t>
   </si>
@@ -1911,33 +1911,15 @@
     <t>Measure/Variable Unique Name</t>
   </si>
   <si>
-    <t>standard_report_legacy.total_natural_gas</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.total_electricity</t>
-  </si>
-  <si>
     <t>standard_report_legacy.total_energy</t>
   </si>
   <si>
-    <t>standard_report_legacy.total_source_energy</t>
-  </si>
-  <si>
     <t>Taxonomy Identifier</t>
   </si>
   <si>
     <t>total_site_energy_intensity</t>
   </si>
   <si>
-    <t>total_source_energy_intensity</t>
-  </si>
-  <si>
-    <t>total_electricity_intensity</t>
-  </si>
-  <si>
-    <t>total_natural_gas_intensity</t>
-  </si>
-  <si>
     <t>Machine Name thats Link to Dencity Taxonomy</t>
   </si>
   <si>
@@ -1947,15 +1929,6 @@
     <t>Total Site Energy Intensity</t>
   </si>
   <si>
-    <t>Total Source Energy Intensity</t>
-  </si>
-  <si>
-    <t>Total Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>Total Electricity Intensity</t>
-  </si>
-  <si>
     <t>OSM</t>
   </si>
   <si>
@@ -2064,120 +2037,6 @@
     <t>Space Infiltration Reduction</t>
   </si>
   <si>
-    <t>Natural Gas Heating Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heating_natural_gas</t>
-  </si>
-  <si>
-    <t>Cooling Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.cooling_electricity</t>
-  </si>
-  <si>
-    <t>Interior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Exterior Lighting Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_lighting_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Equipment Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.interior_equipment_natural_gas</t>
-  </si>
-  <si>
-    <t>Experior Equipment Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.exterior_equipment_electricity</t>
-  </si>
-  <si>
-    <t>Fans Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.fans_electricity</t>
-  </si>
-  <si>
-    <t>Pumps Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.pumps_electricity</t>
-  </si>
-  <si>
-    <t>Heat Rejection Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.heat_rejection_electricity</t>
-  </si>
-  <si>
-    <t>Humidification Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.humidification_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_electricity</t>
-  </si>
-  <si>
-    <t>Water Systems Natural Gas Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.water_systems_natural_gas</t>
-  </si>
-  <si>
-    <t>Refrigeration Electricity Intensity</t>
-  </si>
-  <si>
-    <t>standard_report_legacy.refrigeration_electricity</t>
-  </si>
-  <si>
-    <t>Unmet Cooling Hours</t>
-  </si>
-  <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_cooling</t>
-  </si>
-  <si>
-    <t>hrs</t>
-  </si>
-  <si>
-    <t>Unmet Heating Hours</t>
-  </si>
-  <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_heating</t>
-  </si>
-  <si>
-    <t>Total Unmet Hours</t>
-  </si>
-  <si>
-    <t>standard_report.time_setpoint_not_met_during_occupied_hours</t>
-  </si>
-  <si>
-    <t>Building Area</t>
-  </si>
-  <si>
-    <t>standard_report.total_building_area</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
     <t>Electric RMSE</t>
   </si>
   <si>
@@ -2344,12 +2203,6 @@
   </si>
   <si>
     <t>Short display names are used for plots and exported to metadata</t>
-  </si>
-  <si>
-    <t>NG EUI</t>
-  </si>
-  <si>
-    <t>Elec EUI</t>
   </si>
   <si>
     <t>../Calibration_example/measures</t>
@@ -4523,7 +4376,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -4585,7 +4438,6 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -6789,7 +6641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
@@ -6826,7 +6678,7 @@
         <v>434</v>
       </c>
       <c r="B3" s="25" t="s">
-        <v>764</v>
+        <v>717</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>435</v>
@@ -6837,7 +6689,7 @@
         <v>454</v>
       </c>
       <c r="B4" s="24" t="s">
-        <v>774</v>
+        <v>725</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>455</v>
@@ -6848,7 +6700,7 @@
         <v>465</v>
       </c>
       <c r="B5" s="25" t="s">
-        <v>804</v>
+        <v>755</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>609</v>
@@ -6859,7 +6711,7 @@
         <v>466</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>801</v>
+        <v>752</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>468</v>
@@ -6872,11 +6724,11 @@
       <c r="B7" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="C7" s="32" t="str">
+      <c r="C7" s="31" t="str">
         <f>VLOOKUP($B7,instance_defs,2,FALSE)&amp;VLOOKUP($B7,instance_defs,4,FALSE)</f>
         <v>16 Cores - Worker Only - Recommended for Worker</v>
       </c>
-      <c r="D7" s="32" t="str">
+      <c r="D7" s="31" t="str">
         <f>VLOOKUP($B7,instance_defs,3,FALSE)</f>
         <v>$1.68/hour</v>
       </c>
@@ -6891,11 +6743,11 @@
       <c r="B8" s="24" t="s">
         <v>599</v>
       </c>
-      <c r="C8" s="32" t="str">
+      <c r="C8" s="31" t="str">
         <f>VLOOKUP($B8,instance_defs,2,FALSE)&amp;VLOOKUP($B8,instance_defs,4,FALSE)</f>
         <v>16 Cores - Worker Only - Recommended for Worker</v>
       </c>
-      <c r="D8" s="32" t="str">
+      <c r="D8" s="31" t="str">
         <f>VLOOKUP($B8,instance_defs,3,FALSE)</f>
         <v>$1.68/hour</v>
       </c>
@@ -6911,7 +6763,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="32"/>
+      <c r="D9" s="31"/>
       <c r="E9" s="2" t="s">
         <v>602</v>
       </c>
@@ -6930,7 +6782,7 @@
         <v>38</v>
       </c>
       <c r="B12" s="24" t="s">
-        <v>763</v>
+        <v>716</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>467</v>
@@ -6941,10 +6793,10 @@
         <v>24</v>
       </c>
       <c r="B13" s="24" t="s">
-        <v>770</v>
+        <v>721</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -6952,10 +6804,10 @@
         <v>25</v>
       </c>
       <c r="B14" s="24" t="s">
-        <v>736</v>
+        <v>689</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>647</v>
+        <v>638</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -7032,7 +6884,7 @@
       <c r="C22" s="29" t="s">
         <v>575</v>
       </c>
-      <c r="D22" s="34"/>
+      <c r="D22" s="33"/>
     </row>
     <row r="23" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="30" t="s">
@@ -7044,7 +6896,7 @@
       <c r="C23" s="29" t="s">
         <v>574</v>
       </c>
-      <c r="D23" s="34"/>
+      <c r="D23" s="33"/>
     </row>
     <row r="24" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="30" t="s">
@@ -7056,7 +6908,7 @@
       <c r="C24" s="29" t="s">
         <v>580</v>
       </c>
-      <c r="D24" s="34"/>
+      <c r="D24" s="33"/>
     </row>
     <row r="25" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="30" t="s">
@@ -7068,7 +6920,7 @@
       <c r="C25" s="29" t="s">
         <v>582</v>
       </c>
-      <c r="D25" s="34"/>
+      <c r="D25" s="33"/>
     </row>
     <row r="26" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="30" t="s">
@@ -7080,7 +6932,7 @@
       <c r="C26" s="29" t="s">
         <v>583</v>
       </c>
-      <c r="D26" s="34"/>
+      <c r="D26" s="33"/>
     </row>
     <row r="27" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="30" t="s">
@@ -7092,7 +6944,7 @@
       <c r="C27" s="29" t="s">
         <v>581</v>
       </c>
-      <c r="D27" s="34"/>
+      <c r="D27" s="33"/>
     </row>
     <row r="28" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="30" t="s">
@@ -7102,7 +6954,7 @@
         <v>536</v>
       </c>
       <c r="C28" s="29"/>
-      <c r="D28" s="34"/>
+      <c r="D28" s="33"/>
     </row>
     <row r="29" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="30" t="s">
@@ -7114,31 +6966,31 @@
       <c r="C29" s="29" t="s">
         <v>569</v>
       </c>
-      <c r="D29" s="34"/>
+      <c r="D29" s="33"/>
     </row>
     <row r="30" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="30" t="s">
-        <v>737</v>
+        <v>690</v>
       </c>
       <c r="B30" s="29">
         <v>0</v>
       </c>
-      <c r="C30" s="33" t="s">
-        <v>738</v>
-      </c>
-      <c r="D30" s="34"/>
+      <c r="C30" s="32" t="s">
+        <v>691</v>
+      </c>
+      <c r="D30" s="33"/>
     </row>
     <row r="31" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
-      <c r="D31" s="34"/>
+      <c r="D31" s="33"/>
     </row>
     <row r="32" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
-      <c r="D32" s="34"/>
+      <c r="D32" s="33"/>
     </row>
     <row r="33" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
       <c r="D33" s="2"/>
@@ -7148,7 +7000,7 @@
         <v>32</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="C34" s="11" t="s">
         <v>30</v>
@@ -7161,7 +7013,7 @@
         <v>28</v>
       </c>
       <c r="B35" s="24" t="s">
-        <v>771</v>
+        <v>722</v>
       </c>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
@@ -7175,7 +7027,7 @@
         <v>37</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="E37" s="13" t="s">
         <v>447</v>
@@ -7186,10 +7038,10 @@
         <v>31</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>638</v>
+        <v>629</v>
       </c>
       <c r="D38" s="30" t="s">
-        <v>772</v>
+        <v>723</v>
       </c>
       <c r="E38" s="2"/>
     </row>
@@ -7201,7 +7053,7 @@
         <v>33</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>648</v>
+        <v>639</v>
       </c>
       <c r="D40" s="11"/>
       <c r="E40" s="13" t="s">
@@ -7210,13 +7062,13 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="30" t="s">
-        <v>641</v>
+        <v>632</v>
       </c>
       <c r="B41" s="25" t="s">
-        <v>640</v>
+        <v>631</v>
       </c>
       <c r="C41" s="30" t="s">
-        <v>773</v>
+        <v>724</v>
       </c>
     </row>
     <row r="42" spans="1:5" s="30" customFormat="1" x14ac:dyDescent="0.3">
@@ -7284,7 +7136,7 @@
         <v>39</v>
       </c>
       <c r="E1" s="5"/>
-      <c r="F1" s="59"/>
+      <c r="F1" s="58"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6"/>
@@ -7296,21 +7148,21 @@
       <c r="M1" s="22"/>
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
-      <c r="P1" s="35" t="s">
+      <c r="P1" s="34" t="s">
         <v>470</v>
       </c>
       <c r="Q1" s="23"/>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
-      <c r="U1" s="65" t="s">
+      <c r="U1" s="64" t="s">
         <v>59</v>
       </c>
-      <c r="V1" s="65"/>
-      <c r="W1" s="65"/>
-      <c r="X1" s="65"/>
-      <c r="Y1" s="65"/>
-      <c r="Z1" s="65"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
     </row>
     <row r="2" spans="1:26" s="8" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -7325,7 +7177,7 @@
       <c r="D2" s="8" t="s">
         <v>541</v>
       </c>
-      <c r="F2" s="60"/>
+      <c r="F2" s="59"/>
       <c r="I2" s="9"/>
       <c r="J2" s="9"/>
     </row>
@@ -7345,8 +7197,8 @@
       <c r="E3" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="61" t="s">
-        <v>765</v>
+      <c r="F3" s="60" t="s">
+        <v>718</v>
       </c>
       <c r="G3" s="15" t="s">
         <v>11</v>
@@ -7406,41 +7258,41 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="b">
+    <row r="4" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>797</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>775</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>775</v>
-      </c>
-      <c r="E4" s="36" t="s">
+      <c r="B4" s="35" t="s">
+        <v>748</v>
+      </c>
+      <c r="C4" s="35" t="s">
+        <v>726</v>
+      </c>
+      <c r="D4" s="35" t="s">
+        <v>726</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="H4" s="37"/>
-      <c r="I4" s="37"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B5" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>776</v>
+        <v>727</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>777</v>
-      </c>
-      <c r="F5" s="62"/>
+        <v>728</v>
+      </c>
+      <c r="F5" s="61"/>
       <c r="G5" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I5" s="30" t="s">
-        <v>778</v>
+        <v>729</v>
       </c>
       <c r="J5" s="30"/>
     </row>
@@ -7449,17 +7301,17 @@
         <v>21</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>779</v>
+        <v>730</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="F6" s="62"/>
+      <c r="F6" s="61"/>
       <c r="G6" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>780</v>
+        <v>731</v>
       </c>
       <c r="J6" s="30"/>
     </row>
@@ -7468,17 +7320,17 @@
         <v>21</v>
       </c>
       <c r="D7" s="30" t="s">
-        <v>781</v>
+        <v>732</v>
       </c>
       <c r="E7" s="30" t="s">
-        <v>782</v>
-      </c>
-      <c r="F7" s="62"/>
+        <v>733</v>
+      </c>
+      <c r="F7" s="61"/>
       <c r="G7" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I7" s="30" t="s">
-        <v>783</v>
+        <v>734</v>
       </c>
       <c r="J7" s="30"/>
     </row>
@@ -7487,17 +7339,17 @@
         <v>21</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>784</v>
+        <v>735</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>785</v>
-      </c>
-      <c r="F8" s="62"/>
+        <v>736</v>
+      </c>
+      <c r="F8" s="61"/>
       <c r="G8" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I8" s="30" t="s">
-        <v>643</v>
+        <v>634</v>
       </c>
       <c r="J8" s="30"/>
     </row>
@@ -7506,17 +7358,17 @@
         <v>21</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>786</v>
+        <v>737</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="F9" s="62"/>
+        <v>738</v>
+      </c>
+      <c r="F9" s="61"/>
       <c r="G9" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I9" s="30" t="s">
-        <v>788</v>
+        <v>739</v>
       </c>
       <c r="J9" s="30"/>
     </row>
@@ -7525,17 +7377,17 @@
         <v>21</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>719</v>
+        <v>672</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>720</v>
-      </c>
-      <c r="F10" s="62"/>
+        <v>673</v>
+      </c>
+      <c r="F10" s="61"/>
       <c r="G10" s="30" t="s">
-        <v>718</v>
-      </c>
-      <c r="I10" s="47" t="s">
-        <v>747</v>
+        <v>671</v>
+      </c>
+      <c r="I10" s="46" t="s">
+        <v>700</v>
       </c>
       <c r="J10" s="30"/>
     </row>
@@ -7544,17 +7396,17 @@
         <v>21</v>
       </c>
       <c r="D11" s="30" t="s">
-        <v>721</v>
+        <v>674</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>722</v>
-      </c>
-      <c r="F11" s="62"/>
+        <v>675</v>
+      </c>
+      <c r="F11" s="61"/>
       <c r="G11" s="30" t="s">
-        <v>718</v>
-      </c>
-      <c r="I11" s="47" t="s">
-        <v>748</v>
+        <v>671</v>
+      </c>
+      <c r="I11" s="46" t="s">
+        <v>701</v>
       </c>
       <c r="J11" s="30"/>
     </row>
@@ -7563,17 +7415,17 @@
         <v>21</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>789</v>
+        <v>740</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>790</v>
-      </c>
-      <c r="F12" s="62"/>
+        <v>741</v>
+      </c>
+      <c r="F12" s="61"/>
       <c r="G12" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="47" t="s">
-        <v>791</v>
+      <c r="I12" s="46" t="s">
+        <v>742</v>
       </c>
       <c r="J12" s="30"/>
     </row>
@@ -7582,55 +7434,55 @@
         <v>21</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>799</v>
+        <v>750</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>800</v>
-      </c>
-      <c r="F13" s="62"/>
+        <v>751</v>
+      </c>
+      <c r="F13" s="61"/>
       <c r="G13" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="I13" s="47" t="s">
-        <v>791</v>
+      <c r="I13" s="46" t="s">
+        <v>742</v>
       </c>
       <c r="J13" s="30"/>
     </row>
-    <row r="14" spans="1:26" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="36" t="b">
+    <row r="14" spans="1:26" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="B14" s="36" t="s">
-        <v>798</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>775</v>
-      </c>
-      <c r="D14" s="36" t="s">
-        <v>775</v>
-      </c>
-      <c r="E14" s="36" t="s">
+      <c r="B14" s="35" t="s">
+        <v>749</v>
+      </c>
+      <c r="C14" s="35" t="s">
+        <v>726</v>
+      </c>
+      <c r="D14" s="35" t="s">
+        <v>726</v>
+      </c>
+      <c r="E14" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="37"/>
-      <c r="I14" s="37"/>
+      <c r="H14" s="36"/>
+      <c r="I14" s="36"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B15" s="30" t="s">
         <v>21</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>776</v>
+        <v>727</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>777</v>
-      </c>
-      <c r="F15" s="62"/>
+        <v>728</v>
+      </c>
+      <c r="F15" s="61"/>
       <c r="G15" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I15" s="30" t="s">
-        <v>792</v>
+        <v>743</v>
       </c>
       <c r="J15" s="30"/>
     </row>
@@ -7639,17 +7491,17 @@
         <v>21</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>779</v>
+        <v>730</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>164</v>
       </c>
-      <c r="F16" s="62"/>
+      <c r="F16" s="61"/>
       <c r="G16" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I16" s="30" t="s">
-        <v>793</v>
+        <v>744</v>
       </c>
       <c r="J16" s="30"/>
     </row>
@@ -7658,17 +7510,17 @@
         <v>21</v>
       </c>
       <c r="D17" s="30" t="s">
-        <v>781</v>
+        <v>732</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>782</v>
-      </c>
-      <c r="F17" s="62"/>
+        <v>733</v>
+      </c>
+      <c r="F17" s="61"/>
       <c r="G17" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I17" s="30" t="s">
-        <v>794</v>
+        <v>745</v>
       </c>
       <c r="J17" s="30"/>
     </row>
@@ -7677,17 +7529,17 @@
         <v>21</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>784</v>
+        <v>735</v>
       </c>
       <c r="E18" s="30" t="s">
-        <v>785</v>
-      </c>
-      <c r="F18" s="62"/>
+        <v>736</v>
+      </c>
+      <c r="F18" s="61"/>
       <c r="G18" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I18" s="30" t="s">
-        <v>645</v>
+        <v>636</v>
       </c>
       <c r="J18" s="30"/>
     </row>
@@ -7696,17 +7548,17 @@
         <v>21</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>786</v>
+        <v>737</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>787</v>
-      </c>
-      <c r="F19" s="62"/>
+        <v>738</v>
+      </c>
+      <c r="F19" s="61"/>
       <c r="G19" s="30" t="s">
-        <v>718</v>
+        <v>671</v>
       </c>
       <c r="I19" s="30" t="s">
-        <v>795</v>
+        <v>746</v>
       </c>
       <c r="J19" s="30"/>
     </row>
@@ -7715,17 +7567,17 @@
         <v>21</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>719</v>
+        <v>672</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>720</v>
-      </c>
-      <c r="F20" s="62"/>
+        <v>673</v>
+      </c>
+      <c r="F20" s="61"/>
       <c r="G20" s="30" t="s">
-        <v>718</v>
-      </c>
-      <c r="I20" s="47" t="s">
-        <v>747</v>
+        <v>671</v>
+      </c>
+      <c r="I20" s="46" t="s">
+        <v>700</v>
       </c>
       <c r="J20" s="30"/>
     </row>
@@ -7734,17 +7586,17 @@
         <v>21</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>721</v>
+        <v>674</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>722</v>
-      </c>
-      <c r="F21" s="62"/>
+        <v>675</v>
+      </c>
+      <c r="F21" s="61"/>
       <c r="G21" s="30" t="s">
-        <v>718</v>
-      </c>
-      <c r="I21" s="47" t="s">
-        <v>748</v>
+        <v>671</v>
+      </c>
+      <c r="I21" s="46" t="s">
+        <v>701</v>
       </c>
       <c r="J21" s="30"/>
     </row>
@@ -7753,53 +7605,53 @@
         <v>21</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>789</v>
+        <v>740</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>790</v>
-      </c>
-      <c r="F22" s="62"/>
+        <v>741</v>
+      </c>
+      <c r="F22" s="61"/>
       <c r="G22" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="47" t="s">
-        <v>796</v>
+      <c r="I22" s="46" t="s">
+        <v>747</v>
       </c>
       <c r="J22" s="30"/>
     </row>
-    <row r="23" spans="1:18" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="36" t="b">
+    <row r="23" spans="1:18" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="35" t="b">
         <v>1</v>
       </c>
-      <c r="B23" s="36" t="s">
-        <v>802</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>805</v>
-      </c>
-      <c r="D23" s="36" t="s">
-        <v>805</v>
-      </c>
-      <c r="E23" s="36" t="s">
+      <c r="B23" s="35" t="s">
+        <v>753</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>756</v>
+      </c>
+      <c r="D23" s="35" t="s">
+        <v>756</v>
+      </c>
+      <c r="E23" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-    </row>
-    <row r="24" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="44" t="b">
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+    </row>
+    <row r="24" spans="1:18" s="43" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="43" t="b">
         <v>1</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="B24" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="C24" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="D24" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>66</v>
       </c>
     </row>
@@ -7813,7 +7665,7 @@
       <c r="E25" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="61"/>
       <c r="G25" s="29" t="s">
         <v>60</v>
       </c>
@@ -7825,41 +7677,41 @@
       </c>
       <c r="P25" s="30"/>
     </row>
-    <row r="26" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B26" s="39" t="s">
+    <row r="26" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B26" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="40" t="s">
-        <v>673</v>
-      </c>
-      <c r="E26" s="39" t="s">
+      <c r="D26" s="39" t="s">
+        <v>664</v>
+      </c>
+      <c r="E26" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="49"/>
-      <c r="G26" s="39" t="s">
+      <c r="F26" s="48"/>
+      <c r="G26" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="I26" s="39">
-        <v>0</v>
-      </c>
-      <c r="K26" s="41">
-        <v>0</v>
-      </c>
-      <c r="L26" s="41">
+      <c r="I26" s="38">
+        <v>0</v>
+      </c>
+      <c r="K26" s="40">
+        <v>0</v>
+      </c>
+      <c r="L26" s="40">
         <v>100</v>
       </c>
-      <c r="M26" s="41">
+      <c r="M26" s="40">
         <v>15</v>
       </c>
-      <c r="N26" s="41">
+      <c r="N26" s="40">
         <f>(L26-K26)/6</f>
         <v>16.666666666666668</v>
       </c>
-      <c r="O26" s="41">
+      <c r="O26" s="40">
         <v>1</v>
       </c>
-      <c r="R26" s="39" t="s">
-        <v>803</v>
+      <c r="R26" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="27" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7867,12 +7719,12 @@
         <v>21</v>
       </c>
       <c r="D27" s="29" t="s">
-        <v>665</v>
+        <v>656</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>666</v>
-      </c>
-      <c r="F27" s="62"/>
+        <v>657</v>
+      </c>
+      <c r="F27" s="61"/>
       <c r="G27" s="29" t="s">
         <v>62</v>
       </c>
@@ -7880,41 +7732,41 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D28" s="56" t="s">
-        <v>668</v>
-      </c>
-      <c r="E28" s="55" t="s">
-        <v>667</v>
-      </c>
-      <c r="F28" s="62"/>
-      <c r="G28" s="55" t="s">
+    <row r="28" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" s="55" t="s">
+        <v>659</v>
+      </c>
+      <c r="E28" s="54" t="s">
+        <v>658</v>
+      </c>
+      <c r="F28" s="61"/>
+      <c r="G28" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="I28" s="55">
-        <v>0</v>
-      </c>
-      <c r="K28" s="57">
-        <v>0</v>
-      </c>
-      <c r="L28" s="57">
+      <c r="I28" s="54">
+        <v>0</v>
+      </c>
+      <c r="K28" s="56">
+        <v>0</v>
+      </c>
+      <c r="L28" s="56">
         <v>0.1</v>
       </c>
-      <c r="M28" s="57">
+      <c r="M28" s="56">
         <v>0.05</v>
       </c>
-      <c r="N28" s="57">
+      <c r="N28" s="56">
         <f>(L28-K28)/6</f>
         <v>1.6666666666666666E-2</v>
       </c>
-      <c r="O28" s="57">
+      <c r="O28" s="56">
         <v>0.01</v>
       </c>
-      <c r="R28" s="55" t="s">
-        <v>803</v>
+      <c r="R28" s="54" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="29" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -7922,12 +7774,12 @@
         <v>21</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>670</v>
+        <v>661</v>
       </c>
       <c r="E29" s="29" t="s">
-        <v>669</v>
-      </c>
-      <c r="F29" s="62"/>
+        <v>660</v>
+      </c>
+      <c r="F29" s="61"/>
       <c r="G29" s="29" t="s">
         <v>62</v>
       </c>
@@ -7940,12 +7792,12 @@
         <v>21</v>
       </c>
       <c r="D30" s="29" t="s">
-        <v>672</v>
+        <v>663</v>
       </c>
       <c r="E30" s="29" t="s">
-        <v>671</v>
-      </c>
-      <c r="F30" s="63"/>
+        <v>662</v>
+      </c>
+      <c r="F30" s="62"/>
       <c r="G30" s="29" t="s">
         <v>62</v>
       </c>
@@ -7963,7 +7815,7 @@
       <c r="E31" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F31" s="63"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="29" t="s">
         <v>62</v>
       </c>
@@ -7981,7 +7833,7 @@
       <c r="E32" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F32" s="63"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="29" t="s">
         <v>62</v>
       </c>
@@ -7999,7 +7851,7 @@
       <c r="E33" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F33" s="63"/>
+      <c r="F33" s="62"/>
       <c r="G33" s="29" t="s">
         <v>63</v>
       </c>
@@ -8008,20 +7860,20 @@
       </c>
       <c r="P33" s="30"/>
     </row>
-    <row r="34" spans="1:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="45" t="b">
+    <row r="34" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B34" s="45" t="s">
+      <c r="B34" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C34" s="45" t="s">
+      <c r="C34" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="D34" s="45" t="s">
+      <c r="D34" s="44" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="45" t="s">
+      <c r="E34" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -8037,7 +7889,7 @@
       <c r="E35" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F35" s="63"/>
+      <c r="F35" s="62"/>
       <c r="G35" s="29" t="s">
         <v>60</v>
       </c>
@@ -8053,45 +7905,45 @@
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
-      <c r="Q35" s="38"/>
-    </row>
-    <row r="36" spans="1:18" s="51" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B36" s="51" t="s">
-        <v>21</v>
-      </c>
-      <c r="D36" s="51" t="s">
-        <v>649</v>
-      </c>
-      <c r="E36" s="51" t="s">
+      <c r="Q35" s="37"/>
+    </row>
+    <row r="36" spans="1:18" s="50" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B36" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" s="50" t="s">
+        <v>640</v>
+      </c>
+      <c r="E36" s="50" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="63"/>
-      <c r="G36" s="51" t="s">
+      <c r="F36" s="62"/>
+      <c r="G36" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="I36" s="51">
-        <v>0</v>
-      </c>
-      <c r="J36" s="52"/>
-      <c r="K36" s="53">
+      <c r="I36" s="50">
+        <v>0</v>
+      </c>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52">
         <v>-40</v>
       </c>
-      <c r="L36" s="53">
+      <c r="L36" s="52">
         <v>40</v>
       </c>
-      <c r="M36" s="53">
-        <v>0</v>
-      </c>
-      <c r="N36" s="53">
+      <c r="M36" s="52">
+        <v>0</v>
+      </c>
+      <c r="N36" s="52">
         <f>(L36-K36)/6</f>
         <v>13.333333333333334</v>
       </c>
-      <c r="O36" s="53">
+      <c r="O36" s="52">
         <v>1</v>
       </c>
-      <c r="Q36" s="54"/>
-      <c r="R36" s="51" t="s">
-        <v>803</v>
+      <c r="Q36" s="53"/>
+      <c r="R36" s="50" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
@@ -8100,13 +7952,13 @@
         <v>21</v>
       </c>
       <c r="C37" s="29"/>
-      <c r="D37" s="43" t="s">
+      <c r="D37" s="42" t="s">
         <v>45</v>
       </c>
       <c r="E37" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F37" s="63"/>
+      <c r="F37" s="62"/>
       <c r="G37" s="29" t="s">
         <v>62</v>
       </c>
@@ -8119,7 +7971,7 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-      <c r="Q37" s="38"/>
+      <c r="Q37" s="37"/>
     </row>
     <row r="38" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" s="29"/>
@@ -8133,7 +7985,7 @@
       <c r="E38" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="63"/>
+      <c r="F38" s="62"/>
       <c r="G38" s="29" t="s">
         <v>62</v>
       </c>
@@ -8146,7 +7998,7 @@
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="Q38" s="38"/>
+      <c r="Q38" s="37"/>
     </row>
     <row r="39" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" s="29"/>
@@ -8160,7 +8012,7 @@
       <c r="E39" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="63"/>
+      <c r="F39" s="62"/>
       <c r="G39" s="29" t="s">
         <v>63</v>
       </c>
@@ -8173,7 +8025,7 @@
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="Q39" s="38"/>
+      <c r="Q39" s="37"/>
     </row>
     <row r="40" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" s="29"/>
@@ -8187,7 +8039,7 @@
       <c r="E40" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F40" s="63"/>
+      <c r="F40" s="62"/>
       <c r="G40" s="29" t="s">
         <v>61</v>
       </c>
@@ -8200,7 +8052,7 @@
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="Q40" s="38"/>
+      <c r="Q40" s="37"/>
     </row>
     <row r="41" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" s="29"/>
@@ -8214,7 +8066,7 @@
       <c r="E41" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F41" s="63"/>
+      <c r="F41" s="62"/>
       <c r="G41" s="29" t="s">
         <v>63</v>
       </c>
@@ -8227,7 +8079,7 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="Q41" s="38"/>
+      <c r="Q41" s="37"/>
     </row>
     <row r="42" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" s="29"/>
@@ -8241,7 +8093,7 @@
       <c r="E42" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F42" s="63"/>
+      <c r="F42" s="62"/>
       <c r="G42" s="29" t="s">
         <v>62</v>
       </c>
@@ -8254,7 +8106,7 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="Q42" s="38"/>
+      <c r="Q42" s="37"/>
     </row>
     <row r="43" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" s="29"/>
@@ -8268,7 +8120,7 @@
       <c r="E43" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F43" s="63"/>
+      <c r="F43" s="62"/>
       <c r="G43" s="29" t="s">
         <v>63</v>
       </c>
@@ -8281,22 +8133,22 @@
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="Q43" s="38"/>
-    </row>
-    <row r="44" spans="1:18" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="45" t="b">
+      <c r="Q43" s="37"/>
+    </row>
+    <row r="44" spans="1:18" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="44" t="s">
         <v>283</v>
       </c>
-      <c r="C44" s="45" t="s">
+      <c r="C44" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="D44" s="45" t="s">
+      <c r="D44" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="E44" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -8310,7 +8162,7 @@
       <c r="E45" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F45" s="63"/>
+      <c r="F45" s="62"/>
       <c r="G45" s="29" t="s">
         <v>60</v>
       </c>
@@ -8321,45 +8173,45 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B46" s="39" t="s">
+    <row r="46" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B46" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="D46" s="39" t="s">
-        <v>650</v>
-      </c>
-      <c r="E46" s="39" t="s">
+      <c r="D46" s="38" t="s">
+        <v>641</v>
+      </c>
+      <c r="E46" s="38" t="s">
         <v>286</v>
       </c>
-      <c r="F46" s="49"/>
-      <c r="G46" s="39" t="s">
+      <c r="F46" s="48"/>
+      <c r="G46" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H46" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I46" s="39">
-        <v>0</v>
-      </c>
-      <c r="J46" s="42"/>
-      <c r="K46" s="41">
+      <c r="H46" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I46" s="38">
+        <v>0</v>
+      </c>
+      <c r="J46" s="41"/>
+      <c r="K46" s="40">
         <v>-80</v>
       </c>
-      <c r="L46" s="41">
+      <c r="L46" s="40">
         <v>80</v>
       </c>
-      <c r="M46" s="41">
-        <v>0</v>
-      </c>
-      <c r="N46" s="41">
+      <c r="M46" s="40">
+        <v>0</v>
+      </c>
+      <c r="N46" s="40">
         <f>(L46-K46)/6</f>
         <v>26.666666666666668</v>
       </c>
-      <c r="O46" s="41">
+      <c r="O46" s="40">
         <v>1</v>
       </c>
-      <c r="R46" s="39" t="s">
-        <v>803</v>
+      <c r="R46" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="47" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8367,17 +8219,17 @@
         <v>21</v>
       </c>
       <c r="D47" s="29" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="E47" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="F47" s="63"/>
+      <c r="F47" s="62"/>
       <c r="G47" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H47" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I47" s="29">
         <v>0</v>
@@ -8388,17 +8240,17 @@
         <v>21</v>
       </c>
       <c r="D48" s="29" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="E48" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F48" s="62"/>
+      <c r="F48" s="61"/>
       <c r="G48" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H48" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I48" s="29">
         <v>0</v>
@@ -8409,17 +8261,17 @@
         <v>21</v>
       </c>
       <c r="D49" s="29" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="E49" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F49" s="62"/>
+      <c r="F49" s="61"/>
       <c r="G49" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H49" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I49" s="29">
         <v>0</v>
@@ -8430,12 +8282,12 @@
         <v>21</v>
       </c>
       <c r="D50" s="29" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="E50" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F50" s="62"/>
+      <c r="F50" s="61"/>
       <c r="G50" s="29" t="s">
         <v>61</v>
       </c>
@@ -8448,17 +8300,17 @@
         <v>21</v>
       </c>
       <c r="D51" s="29" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="E51" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F51" s="62"/>
+      <c r="F51" s="61"/>
       <c r="G51" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H51" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I51" s="29">
         <v>15</v>
@@ -8469,17 +8321,17 @@
         <v>21</v>
       </c>
       <c r="D52" s="29" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="E52" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F52" s="62"/>
+      <c r="F52" s="61"/>
       <c r="G52" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H52" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I52" s="29">
         <v>0</v>
@@ -8490,36 +8342,36 @@
         <v>21</v>
       </c>
       <c r="D53" s="29" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="E53" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F53" s="63"/>
+      <c r="F53" s="62"/>
       <c r="G53" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H53" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I53" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="45" t="b">
+    <row r="54" spans="1:18" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B54" s="45" t="s">
-        <v>743</v>
-      </c>
-      <c r="C54" s="45" t="s">
-        <v>744</v>
-      </c>
-      <c r="D54" s="45" t="s">
-        <v>744</v>
-      </c>
-      <c r="E54" s="45" t="s">
+      <c r="B54" s="44" t="s">
+        <v>696</v>
+      </c>
+      <c r="C54" s="44" t="s">
+        <v>697</v>
+      </c>
+      <c r="D54" s="44" t="s">
+        <v>697</v>
+      </c>
+      <c r="E54" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -8533,56 +8385,56 @@
       <c r="E55" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="F55" s="63"/>
+      <c r="F55" s="62"/>
       <c r="G55" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I55" s="50" t="s">
+      <c r="I55" s="49" t="s">
         <v>415</v>
       </c>
       <c r="J55" s="29" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="56" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B56" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D56" s="39" t="s">
-        <v>745</v>
-      </c>
-      <c r="E56" s="39" t="s">
-        <v>746</v>
-      </c>
-      <c r="F56" s="49"/>
-      <c r="G56" s="39" t="s">
+      <c r="D56" s="38" t="s">
+        <v>698</v>
+      </c>
+      <c r="E56" s="38" t="s">
+        <v>699</v>
+      </c>
+      <c r="F56" s="48"/>
+      <c r="G56" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H56" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I56" s="39">
+      <c r="H56" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I56" s="38">
         <v>0.8</v>
       </c>
-      <c r="J56" s="42"/>
-      <c r="K56" s="41">
+      <c r="J56" s="41"/>
+      <c r="K56" s="40">
         <v>0.78</v>
       </c>
-      <c r="L56" s="41">
+      <c r="L56" s="40">
         <v>0.98</v>
       </c>
-      <c r="M56" s="41">
+      <c r="M56" s="40">
         <v>0.8</v>
       </c>
-      <c r="N56" s="41">
+      <c r="N56" s="40">
         <f>(L56-K56)/6</f>
         <v>3.3333333333333326E-2</v>
       </c>
-      <c r="O56" s="41">
+      <c r="O56" s="40">
         <v>1</v>
       </c>
-      <c r="R56" s="39" t="s">
-        <v>803</v>
+      <c r="R56" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="57" spans="1:18" s="29" customFormat="1" x14ac:dyDescent="0.3">
@@ -8608,7 +8460,7 @@
         <v>21</v>
       </c>
       <c r="D58" s="29" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="E58" s="29" t="s">
         <v>126</v>
@@ -8618,7 +8470,7 @@
         <v>62</v>
       </c>
       <c r="H58" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I58" s="29">
         <v>0</v>
@@ -8629,7 +8481,7 @@
         <v>21</v>
       </c>
       <c r="D59" s="29" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="E59" s="29" t="s">
         <v>48</v>
@@ -8639,7 +8491,7 @@
         <v>62</v>
       </c>
       <c r="H59" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I59" s="29">
         <v>0</v>
@@ -8650,7 +8502,7 @@
         <v>21</v>
       </c>
       <c r="D60" s="29" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="E60" s="29" t="s">
         <v>50</v>
@@ -8660,7 +8512,7 @@
         <v>63</v>
       </c>
       <c r="H60" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I60" s="29">
         <v>0</v>
@@ -8671,12 +8523,12 @@
         <v>21</v>
       </c>
       <c r="D61" s="29" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="E61" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F61" s="63"/>
+      <c r="F61" s="62"/>
       <c r="G61" s="29" t="s">
         <v>61</v>
       </c>
@@ -8689,17 +8541,17 @@
         <v>21</v>
       </c>
       <c r="D62" s="29" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="E62" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F62" s="63"/>
+      <c r="F62" s="62"/>
       <c r="G62" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H62" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I62" s="29">
         <v>15</v>
@@ -8710,17 +8562,17 @@
         <v>21</v>
       </c>
       <c r="D63" s="29" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="E63" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F63" s="63"/>
+      <c r="F63" s="62"/>
       <c r="G63" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H63" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I63" s="29">
         <v>0</v>
@@ -8731,36 +8583,36 @@
         <v>21</v>
       </c>
       <c r="D64" s="29" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="E64" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F64" s="63"/>
+      <c r="F64" s="62"/>
       <c r="G64" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H64" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I64" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="45" t="b">
+    <row r="65" spans="1:18" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B65" s="45" t="s">
-        <v>750</v>
-      </c>
-      <c r="C65" s="45" t="s">
-        <v>749</v>
-      </c>
-      <c r="D65" s="45" t="s">
-        <v>749</v>
-      </c>
-      <c r="E65" s="45" t="s">
+      <c r="B65" s="44" t="s">
+        <v>703</v>
+      </c>
+      <c r="C65" s="44" t="s">
+        <v>702</v>
+      </c>
+      <c r="D65" s="44" t="s">
+        <v>702</v>
+      </c>
+      <c r="E65" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -8769,61 +8621,61 @@
         <v>21</v>
       </c>
       <c r="D66" s="29" t="s">
-        <v>751</v>
+        <v>704</v>
       </c>
       <c r="E66" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="F66" s="63"/>
+      <c r="F66" s="62"/>
       <c r="G66" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I66" s="50" t="s">
+      <c r="I66" s="49" t="s">
         <v>415</v>
       </c>
       <c r="J66" s="29" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="67" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B67" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D67" s="39" t="s">
-        <v>752</v>
-      </c>
-      <c r="E67" s="39" t="s">
-        <v>753</v>
-      </c>
-      <c r="F67" s="49"/>
-      <c r="G67" s="39" t="s">
+      <c r="D67" s="38" t="s">
+        <v>705</v>
+      </c>
+      <c r="E67" s="38" t="s">
+        <v>706</v>
+      </c>
+      <c r="F67" s="48"/>
+      <c r="G67" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H67" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I67" s="39">
+      <c r="H67" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I67" s="38">
         <v>4</v>
       </c>
-      <c r="J67" s="42"/>
-      <c r="K67" s="41">
-        <v>2</v>
-      </c>
-      <c r="L67" s="41">
+      <c r="J67" s="41"/>
+      <c r="K67" s="40">
+        <v>2</v>
+      </c>
+      <c r="L67" s="40">
         <v>5</v>
       </c>
-      <c r="M67" s="41">
+      <c r="M67" s="40">
         <v>4</v>
       </c>
-      <c r="N67" s="41">
+      <c r="N67" s="40">
         <f>(L67-K67)/6</f>
         <v>0.5</v>
       </c>
-      <c r="O67" s="41">
+      <c r="O67" s="40">
         <v>0.25</v>
       </c>
-      <c r="R67" s="39" t="s">
-        <v>803</v>
+      <c r="R67" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="68" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -8836,7 +8688,7 @@
       <c r="E68" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F68" s="63"/>
+      <c r="F68" s="62"/>
       <c r="G68" s="29" t="s">
         <v>61</v>
       </c>
@@ -8849,17 +8701,17 @@
         <v>21</v>
       </c>
       <c r="D69" s="29" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="E69" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="F69" s="63"/>
+      <c r="F69" s="62"/>
       <c r="G69" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H69" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I69" s="29">
         <v>0</v>
@@ -8870,17 +8722,17 @@
         <v>21</v>
       </c>
       <c r="D70" s="29" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="E70" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F70" s="63"/>
+      <c r="F70" s="62"/>
       <c r="G70" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H70" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I70" s="29">
         <v>0</v>
@@ -8891,17 +8743,17 @@
         <v>21</v>
       </c>
       <c r="D71" s="29" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="E71" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F71" s="63"/>
+      <c r="F71" s="62"/>
       <c r="G71" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H71" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I71" s="29">
         <v>0</v>
@@ -8912,12 +8764,12 @@
         <v>21</v>
       </c>
       <c r="D72" s="29" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="E72" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F72" s="63"/>
+      <c r="F72" s="62"/>
       <c r="G72" s="29" t="s">
         <v>61</v>
       </c>
@@ -8930,17 +8782,17 @@
         <v>21</v>
       </c>
       <c r="D73" s="29" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="E73" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F73" s="63"/>
+      <c r="F73" s="62"/>
       <c r="G73" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H73" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I73" s="29">
         <v>15</v>
@@ -8951,17 +8803,17 @@
         <v>21</v>
       </c>
       <c r="D74" s="29" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="E74" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F74" s="63"/>
+      <c r="F74" s="62"/>
       <c r="G74" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H74" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I74" s="29">
         <v>0</v>
@@ -8972,36 +8824,36 @@
         <v>21</v>
       </c>
       <c r="D75" s="29" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="E75" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F75" s="63"/>
+      <c r="F75" s="62"/>
       <c r="G75" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H75" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I75" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="45" t="b">
+    <row r="76" spans="1:18" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B76" s="45" t="s">
+      <c r="B76" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="C76" s="45" t="s">
+      <c r="C76" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="D76" s="45" t="s">
+      <c r="D76" s="44" t="s">
         <v>241</v>
       </c>
-      <c r="E76" s="45" t="s">
+      <c r="E76" s="44" t="s">
         <v>66</v>
       </c>
     </row>
@@ -9015,97 +8867,97 @@
       <c r="E77" s="29" t="s">
         <v>124</v>
       </c>
-      <c r="F77" s="63"/>
+      <c r="F77" s="62"/>
       <c r="G77" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I77" s="50" t="s">
+      <c r="I77" s="49" t="s">
         <v>415</v>
       </c>
       <c r="J77" s="29" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="78" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B78" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D78" s="39" t="s">
-        <v>754</v>
-      </c>
-      <c r="E78" s="39" t="s">
+      <c r="D78" s="38" t="s">
+        <v>707</v>
+      </c>
+      <c r="E78" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="F78" s="49"/>
-      <c r="G78" s="39" t="s">
+      <c r="F78" s="48"/>
+      <c r="G78" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H78" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I78" s="39">
-        <v>0</v>
-      </c>
-      <c r="J78" s="42"/>
-      <c r="K78" s="41">
+      <c r="H78" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I78" s="38">
+        <v>0</v>
+      </c>
+      <c r="J78" s="41"/>
+      <c r="K78" s="40">
         <v>-20</v>
       </c>
-      <c r="L78" s="41">
+      <c r="L78" s="40">
         <v>14</v>
       </c>
-      <c r="M78" s="41">
-        <v>0</v>
-      </c>
-      <c r="N78" s="41">
+      <c r="M78" s="40">
+        <v>0</v>
+      </c>
+      <c r="N78" s="40">
         <f>(L78-K78)/6</f>
         <v>5.666666666666667</v>
       </c>
-      <c r="O78" s="41">
+      <c r="O78" s="40">
         <v>1</v>
       </c>
-      <c r="R78" s="39" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="79" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="R78" s="38" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B79" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D79" s="39" t="s">
-        <v>755</v>
-      </c>
-      <c r="E79" s="39" t="s">
-        <v>756</v>
-      </c>
-      <c r="F79" s="49"/>
-      <c r="G79" s="39" t="s">
+      <c r="D79" s="38" t="s">
+        <v>708</v>
+      </c>
+      <c r="E79" s="38" t="s">
+        <v>709</v>
+      </c>
+      <c r="F79" s="48"/>
+      <c r="G79" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H79" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I79" s="39">
-        <v>0</v>
-      </c>
-      <c r="J79" s="42"/>
-      <c r="K79" s="41">
+      <c r="H79" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I79" s="38">
+        <v>0</v>
+      </c>
+      <c r="J79" s="41"/>
+      <c r="K79" s="40">
         <v>-25</v>
       </c>
-      <c r="L79" s="41">
+      <c r="L79" s="40">
         <v>30</v>
       </c>
-      <c r="M79" s="41">
-        <v>0</v>
-      </c>
-      <c r="N79" s="41">
+      <c r="M79" s="40">
+        <v>0</v>
+      </c>
+      <c r="N79" s="40">
         <f>(L79-K79)/6</f>
         <v>9.1666666666666661</v>
       </c>
-      <c r="O79" s="41">
+      <c r="O79" s="40">
         <v>1</v>
       </c>
-      <c r="R79" s="39" t="s">
-        <v>803</v>
+      <c r="R79" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="80" spans="1:18" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
@@ -9118,7 +8970,7 @@
       <c r="E80" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F80" s="63"/>
+      <c r="F80" s="62"/>
       <c r="G80" s="29" t="s">
         <v>61</v>
       </c>
@@ -9131,17 +8983,17 @@
         <v>21</v>
       </c>
       <c r="D81" s="29" t="s">
-        <v>652</v>
+        <v>643</v>
       </c>
       <c r="E81" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="F81" s="63"/>
+      <c r="F81" s="62"/>
       <c r="G81" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H81" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I81" s="29">
         <v>0</v>
@@ -9152,17 +9004,17 @@
         <v>21</v>
       </c>
       <c r="D82" s="29" t="s">
-        <v>653</v>
+        <v>644</v>
       </c>
       <c r="E82" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F82" s="63"/>
+      <c r="F82" s="62"/>
       <c r="G82" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H82" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I82" s="29">
         <v>0</v>
@@ -9173,17 +9025,17 @@
         <v>21</v>
       </c>
       <c r="D83" s="29" t="s">
-        <v>654</v>
+        <v>645</v>
       </c>
       <c r="E83" s="29" t="s">
         <v>50</v>
       </c>
-      <c r="F83" s="63"/>
+      <c r="F83" s="62"/>
       <c r="G83" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H83" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I83" s="29">
         <v>0</v>
@@ -9194,12 +9046,12 @@
         <v>21</v>
       </c>
       <c r="D84" s="29" t="s">
-        <v>656</v>
+        <v>647</v>
       </c>
       <c r="E84" s="29" t="s">
         <v>52</v>
       </c>
-      <c r="F84" s="62"/>
+      <c r="F84" s="61"/>
       <c r="G84" s="29" t="s">
         <v>61</v>
       </c>
@@ -9212,17 +9064,17 @@
         <v>21</v>
       </c>
       <c r="D85" s="29" t="s">
-        <v>657</v>
+        <v>648</v>
       </c>
       <c r="E85" s="29" t="s">
         <v>54</v>
       </c>
-      <c r="F85" s="62"/>
+      <c r="F85" s="61"/>
       <c r="G85" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H85" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I85" s="29">
         <v>15</v>
@@ -9233,17 +9085,17 @@
         <v>21</v>
       </c>
       <c r="D86" s="29" t="s">
-        <v>658</v>
+        <v>649</v>
       </c>
       <c r="E86" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="F86" s="62"/>
+      <c r="F86" s="61"/>
       <c r="G86" s="29" t="s">
         <v>62</v>
       </c>
       <c r="H86" s="29" t="s">
-        <v>651</v>
+        <v>642</v>
       </c>
       <c r="I86" s="29">
         <v>0</v>
@@ -9254,119 +9106,119 @@
         <v>21</v>
       </c>
       <c r="D87" s="29" t="s">
-        <v>659</v>
+        <v>650</v>
       </c>
       <c r="E87" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="F87" s="62"/>
+      <c r="F87" s="61"/>
       <c r="G87" s="29" t="s">
         <v>63</v>
       </c>
       <c r="H87" s="29" t="s">
-        <v>655</v>
+        <v>646</v>
       </c>
       <c r="I87" s="29">
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:20" s="45" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="45" t="b">
+    <row r="88" spans="1:20" s="44" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B88" s="45" t="s">
+      <c r="B88" s="44" t="s">
         <v>185</v>
       </c>
-      <c r="C88" s="45" t="s">
-        <v>660</v>
-      </c>
-      <c r="D88" s="45" t="s">
-        <v>660</v>
-      </c>
-      <c r="E88" s="45" t="s">
+      <c r="C88" s="44" t="s">
+        <v>651</v>
+      </c>
+      <c r="D88" s="44" t="s">
+        <v>651</v>
+      </c>
+      <c r="E88" s="44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="89" spans="1:20" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B89" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D89" s="39" t="s">
-        <v>661</v>
-      </c>
-      <c r="E89" s="39" t="s">
+      <c r="D89" s="38" t="s">
+        <v>652</v>
+      </c>
+      <c r="E89" s="38" t="s">
         <v>188</v>
       </c>
-      <c r="F89" s="49"/>
-      <c r="G89" s="39" t="s">
+      <c r="F89" s="48"/>
+      <c r="G89" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H89" s="39" t="s">
-        <v>662</v>
-      </c>
-      <c r="I89" s="39">
-        <v>0</v>
-      </c>
-      <c r="J89" s="42"/>
-      <c r="K89" s="41">
+      <c r="H89" s="38" t="s">
+        <v>653</v>
+      </c>
+      <c r="I89" s="38">
+        <v>0</v>
+      </c>
+      <c r="J89" s="41"/>
+      <c r="K89" s="40">
         <v>-6</v>
       </c>
-      <c r="L89" s="41">
-        <v>2</v>
-      </c>
-      <c r="M89" s="41">
-        <v>0</v>
-      </c>
-      <c r="N89" s="41">
+      <c r="L89" s="40">
+        <v>2</v>
+      </c>
+      <c r="M89" s="40">
+        <v>0</v>
+      </c>
+      <c r="N89" s="40">
         <f>(L89-K89)/6</f>
         <v>1.3333333333333333</v>
       </c>
-      <c r="O89" s="41">
+      <c r="O89" s="40">
         <v>1</v>
       </c>
-      <c r="R89" s="39" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="90" spans="1:20" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="R89" s="38" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="90" spans="1:20" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B90" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D90" s="39" t="s">
-        <v>663</v>
-      </c>
-      <c r="E90" s="39" t="s">
+      <c r="D90" s="38" t="s">
+        <v>654</v>
+      </c>
+      <c r="E90" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="F90" s="49"/>
-      <c r="G90" s="39" t="s">
+      <c r="F90" s="48"/>
+      <c r="G90" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H90" s="39" t="s">
-        <v>662</v>
-      </c>
-      <c r="I90" s="39">
-        <v>0</v>
-      </c>
-      <c r="J90" s="42"/>
-      <c r="K90" s="41">
+      <c r="H90" s="38" t="s">
+        <v>653</v>
+      </c>
+      <c r="I90" s="38">
+        <v>0</v>
+      </c>
+      <c r="J90" s="41"/>
+      <c r="K90" s="40">
         <v>-6</v>
       </c>
-      <c r="L90" s="41">
+      <c r="L90" s="40">
         <v>3.9</v>
       </c>
-      <c r="M90" s="41">
-        <v>0</v>
-      </c>
-      <c r="N90" s="41">
+      <c r="M90" s="40">
+        <v>0</v>
+      </c>
+      <c r="N90" s="40">
         <f>(L90-K90)/6</f>
         <v>1.6500000000000001</v>
       </c>
-      <c r="O90" s="41">
+      <c r="O90" s="40">
         <v>1</v>
       </c>
-      <c r="R90" s="39" t="s">
-        <v>803</v>
+      <c r="R90" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="91" spans="1:20" x14ac:dyDescent="0.3">
@@ -9374,12 +9226,12 @@
         <v>21</v>
       </c>
       <c r="D91" s="30" t="s">
-        <v>664</v>
+        <v>655</v>
       </c>
       <c r="E91" s="30" t="s">
         <v>192</v>
       </c>
-      <c r="F91" s="62"/>
+      <c r="F91" s="61"/>
       <c r="G91" s="30" t="s">
         <v>61</v>
       </c>
@@ -9393,481 +9245,481 @@
       <c r="O91" s="3"/>
     </row>
     <row r="92" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A92" s="48" t="b">
+      <c r="A92" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="B92" s="48" t="s">
-        <v>729</v>
-      </c>
-      <c r="C92" s="48" t="s">
-        <v>730</v>
-      </c>
-      <c r="D92" s="48" t="s">
-        <v>730</v>
-      </c>
-      <c r="E92" s="45" t="s">
+      <c r="B92" s="47" t="s">
+        <v>682</v>
+      </c>
+      <c r="C92" s="47" t="s">
+        <v>683</v>
+      </c>
+      <c r="D92" s="47" t="s">
+        <v>683</v>
+      </c>
+      <c r="E92" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F92" s="45"/>
-      <c r="G92" s="48"/>
-      <c r="H92" s="48"/>
-      <c r="I92" s="48"/>
-      <c r="J92" s="48"/>
-      <c r="K92" s="48"/>
-      <c r="L92" s="48"/>
-      <c r="M92" s="45"/>
-      <c r="N92" s="45"/>
-      <c r="O92" s="45"/>
-      <c r="P92" s="45"/>
-      <c r="Q92" s="45"/>
-      <c r="R92" s="45"/>
+      <c r="F92" s="44"/>
+      <c r="G92" s="47"/>
+      <c r="H92" s="47"/>
+      <c r="I92" s="47"/>
+      <c r="J92" s="47"/>
+      <c r="K92" s="47"/>
+      <c r="L92" s="47"/>
+      <c r="M92" s="44"/>
+      <c r="N92" s="44"/>
+      <c r="O92" s="44"/>
+      <c r="P92" s="44"/>
+      <c r="Q92" s="44"/>
+      <c r="R92" s="44"/>
     </row>
     <row r="93" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A93" s="39"/>
+      <c r="A93" s="38"/>
       <c r="B93" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C93" s="49"/>
-      <c r="D93" s="49" t="s">
-        <v>723</v>
-      </c>
-      <c r="E93" s="49" t="s">
-        <v>724</v>
-      </c>
-      <c r="F93" s="49"/>
-      <c r="G93" s="49" t="s">
+      <c r="C93" s="48"/>
+      <c r="D93" s="48" t="s">
+        <v>676</v>
+      </c>
+      <c r="E93" s="48" t="s">
+        <v>677</v>
+      </c>
+      <c r="F93" s="48"/>
+      <c r="G93" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H93" s="49"/>
-      <c r="I93" s="49">
+      <c r="H93" s="48"/>
+      <c r="I93" s="48">
         <v>1</v>
       </c>
-      <c r="J93" s="49"/>
-      <c r="K93" s="49">
+      <c r="J93" s="48"/>
+      <c r="K93" s="48">
         <v>0.5</v>
       </c>
-      <c r="L93" s="49">
+      <c r="L93" s="48">
         <v>4.5</v>
       </c>
-      <c r="M93" s="41">
+      <c r="M93" s="40">
         <v>1.75</v>
       </c>
-      <c r="N93" s="39">
+      <c r="N93" s="38">
         <f>1.5/6</f>
         <v>0.25</v>
       </c>
-      <c r="O93" s="49">
+      <c r="O93" s="48">
         <v>0.1</v>
       </c>
-      <c r="P93" s="39"/>
-      <c r="Q93" s="39"/>
-      <c r="R93" s="39" t="s">
-        <v>803</v>
+      <c r="P93" s="38"/>
+      <c r="Q93" s="38"/>
+      <c r="R93" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="94" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A94" s="49"/>
+      <c r="A94" s="48"/>
       <c r="B94" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C94" s="49"/>
-      <c r="D94" s="49" t="s">
-        <v>725</v>
-      </c>
-      <c r="E94" s="49" t="s">
-        <v>726</v>
-      </c>
-      <c r="F94" s="49"/>
-      <c r="G94" s="49" t="s">
+      <c r="C94" s="48"/>
+      <c r="D94" s="48" t="s">
+        <v>678</v>
+      </c>
+      <c r="E94" s="48" t="s">
+        <v>679</v>
+      </c>
+      <c r="F94" s="48"/>
+      <c r="G94" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H94" s="49"/>
-      <c r="I94" s="49">
+      <c r="H94" s="48"/>
+      <c r="I94" s="48">
         <v>1</v>
       </c>
-      <c r="J94" s="49"/>
-      <c r="K94" s="49">
+      <c r="J94" s="48"/>
+      <c r="K94" s="48">
         <v>0.1</v>
       </c>
-      <c r="L94" s="49">
+      <c r="L94" s="48">
         <v>4.5</v>
       </c>
-      <c r="M94" s="41">
+      <c r="M94" s="40">
         <v>1.75</v>
       </c>
-      <c r="N94" s="49">
+      <c r="N94" s="48">
         <v>0.25</v>
       </c>
-      <c r="O94" s="49">
+      <c r="O94" s="48">
         <v>0.1</v>
       </c>
-      <c r="P94" s="39"/>
-      <c r="Q94" s="39"/>
-      <c r="R94" s="39" t="s">
-        <v>803</v>
+      <c r="P94" s="38"/>
+      <c r="Q94" s="38"/>
+      <c r="R94" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="95" spans="1:20" s="29" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A95" s="49"/>
+      <c r="A95" s="48"/>
       <c r="B95" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49" t="s">
-        <v>727</v>
-      </c>
-      <c r="E95" s="49" t="s">
-        <v>728</v>
-      </c>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49" t="s">
+      <c r="C95" s="48"/>
+      <c r="D95" s="48" t="s">
+        <v>680</v>
+      </c>
+      <c r="E95" s="48" t="s">
+        <v>681</v>
+      </c>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H95" s="49"/>
-      <c r="I95" s="49">
+      <c r="H95" s="48"/>
+      <c r="I95" s="48">
         <v>1</v>
       </c>
-      <c r="J95" s="49"/>
-      <c r="K95" s="49">
+      <c r="J95" s="48"/>
+      <c r="K95" s="48">
         <v>0.5</v>
       </c>
-      <c r="L95" s="49">
+      <c r="L95" s="48">
         <v>3</v>
       </c>
-      <c r="M95" s="41">
+      <c r="M95" s="40">
         <v>1.75</v>
       </c>
-      <c r="N95" s="41">
+      <c r="N95" s="40">
         <v>0.25</v>
       </c>
-      <c r="O95" s="41">
+      <c r="O95" s="40">
         <v>0.1</v>
       </c>
-      <c r="P95" s="41"/>
-      <c r="Q95" s="41"/>
-      <c r="R95" s="39" t="s">
-        <v>803</v>
+      <c r="P95" s="40"/>
+      <c r="Q95" s="40"/>
+      <c r="R95" s="38" t="s">
+        <v>754</v>
       </c>
       <c r="T95" s="30"/>
     </row>
     <row r="96" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A96" s="48" t="b">
+      <c r="A96" s="47" t="b">
         <v>1</v>
       </c>
-      <c r="B96" s="48" t="s">
-        <v>731</v>
-      </c>
-      <c r="C96" s="48" t="s">
-        <v>732</v>
-      </c>
-      <c r="D96" s="48" t="s">
-        <v>732</v>
-      </c>
-      <c r="E96" s="45" t="s">
+      <c r="B96" s="47" t="s">
+        <v>684</v>
+      </c>
+      <c r="C96" s="47" t="s">
+        <v>685</v>
+      </c>
+      <c r="D96" s="47" t="s">
+        <v>685</v>
+      </c>
+      <c r="E96" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="F96" s="45"/>
-      <c r="G96" s="48"/>
-      <c r="H96" s="48"/>
-      <c r="I96" s="48"/>
-      <c r="J96" s="48"/>
-      <c r="K96" s="48"/>
-      <c r="L96" s="48"/>
-      <c r="M96" s="45"/>
-      <c r="N96" s="45"/>
-      <c r="O96" s="45"/>
-      <c r="P96" s="45"/>
-      <c r="Q96" s="45"/>
-      <c r="R96" s="45"/>
+      <c r="F96" s="44"/>
+      <c r="G96" s="47"/>
+      <c r="H96" s="47"/>
+      <c r="I96" s="47"/>
+      <c r="J96" s="47"/>
+      <c r="K96" s="47"/>
+      <c r="L96" s="47"/>
+      <c r="M96" s="44"/>
+      <c r="N96" s="44"/>
+      <c r="O96" s="44"/>
+      <c r="P96" s="44"/>
+      <c r="Q96" s="44"/>
+      <c r="R96" s="44"/>
     </row>
     <row r="97" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A97" s="39"/>
+      <c r="A97" s="38"/>
       <c r="B97" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C97" s="49"/>
-      <c r="D97" s="49" t="s">
-        <v>733</v>
-      </c>
-      <c r="E97" s="49" t="s">
-        <v>724</v>
-      </c>
-      <c r="F97" s="49"/>
-      <c r="G97" s="49" t="s">
+      <c r="C97" s="48"/>
+      <c r="D97" s="48" t="s">
+        <v>686</v>
+      </c>
+      <c r="E97" s="48" t="s">
+        <v>677</v>
+      </c>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H97" s="49"/>
-      <c r="I97" s="49">
+      <c r="H97" s="48"/>
+      <c r="I97" s="48">
         <v>1</v>
       </c>
-      <c r="J97" s="49"/>
-      <c r="K97" s="49">
+      <c r="J97" s="48"/>
+      <c r="K97" s="48">
         <v>0.5</v>
       </c>
-      <c r="L97" s="49">
+      <c r="L97" s="48">
         <v>4</v>
       </c>
-      <c r="M97" s="41">
+      <c r="M97" s="40">
         <v>1.75</v>
       </c>
-      <c r="N97" s="39">
+      <c r="N97" s="38">
         <f>1.5/6</f>
         <v>0.25</v>
       </c>
-      <c r="O97" s="49">
+      <c r="O97" s="48">
         <v>0.1</v>
       </c>
-      <c r="P97" s="39"/>
-      <c r="Q97" s="39"/>
-      <c r="R97" s="39" t="s">
-        <v>803</v>
+      <c r="P97" s="38"/>
+      <c r="Q97" s="38"/>
+      <c r="R97" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="98" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A98" s="49"/>
+      <c r="A98" s="48"/>
       <c r="B98" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C98" s="49"/>
-      <c r="D98" s="49" t="s">
-        <v>734</v>
-      </c>
-      <c r="E98" s="49" t="s">
-        <v>726</v>
-      </c>
-      <c r="F98" s="49"/>
-      <c r="G98" s="49" t="s">
+      <c r="C98" s="48"/>
+      <c r="D98" s="48" t="s">
+        <v>687</v>
+      </c>
+      <c r="E98" s="48" t="s">
+        <v>679</v>
+      </c>
+      <c r="F98" s="48"/>
+      <c r="G98" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H98" s="49"/>
-      <c r="I98" s="49">
+      <c r="H98" s="48"/>
+      <c r="I98" s="48">
         <v>1</v>
       </c>
-      <c r="J98" s="49"/>
-      <c r="K98" s="49">
+      <c r="J98" s="48"/>
+      <c r="K98" s="48">
         <v>0.5</v>
       </c>
-      <c r="L98" s="49">
+      <c r="L98" s="48">
         <v>4</v>
       </c>
-      <c r="M98" s="41">
+      <c r="M98" s="40">
         <v>1.75</v>
       </c>
-      <c r="N98" s="49">
+      <c r="N98" s="48">
         <v>0.25</v>
       </c>
-      <c r="O98" s="49">
+      <c r="O98" s="48">
         <v>0.1</v>
       </c>
-      <c r="P98" s="39"/>
-      <c r="Q98" s="39"/>
-      <c r="R98" s="39" t="s">
-        <v>803</v>
+      <c r="P98" s="38"/>
+      <c r="Q98" s="38"/>
+      <c r="R98" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="99" spans="1:18" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A99" s="49"/>
+      <c r="A99" s="48"/>
       <c r="B99" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C99" s="49"/>
-      <c r="D99" s="49" t="s">
-        <v>735</v>
-      </c>
-      <c r="E99" s="49" t="s">
-        <v>728</v>
-      </c>
-      <c r="F99" s="49"/>
-      <c r="G99" s="49" t="s">
+      <c r="C99" s="48"/>
+      <c r="D99" s="48" t="s">
+        <v>688</v>
+      </c>
+      <c r="E99" s="48" t="s">
+        <v>681</v>
+      </c>
+      <c r="F99" s="48"/>
+      <c r="G99" s="48" t="s">
         <v>62</v>
       </c>
-      <c r="H99" s="49"/>
-      <c r="I99" s="49">
+      <c r="H99" s="48"/>
+      <c r="I99" s="48">
         <v>1</v>
       </c>
-      <c r="J99" s="49"/>
-      <c r="K99" s="49">
+      <c r="J99" s="48"/>
+      <c r="K99" s="48">
         <v>0.5</v>
       </c>
-      <c r="L99" s="49">
+      <c r="L99" s="48">
         <v>3</v>
       </c>
-      <c r="M99" s="41">
+      <c r="M99" s="40">
         <v>1.75</v>
       </c>
-      <c r="N99" s="41">
+      <c r="N99" s="40">
         <v>0.25</v>
       </c>
-      <c r="O99" s="41">
+      <c r="O99" s="40">
         <v>0.1</v>
       </c>
-      <c r="P99" s="41"/>
-      <c r="Q99" s="41"/>
-      <c r="R99" s="39" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="100" spans="1:18" s="45" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A100" s="45" t="b">
+      <c r="P99" s="40"/>
+      <c r="Q99" s="40"/>
+      <c r="R99" s="38" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="100" spans="1:18" s="44" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A100" s="44" t="b">
         <v>1</v>
       </c>
-      <c r="B100" s="45" t="s">
-        <v>758</v>
-      </c>
-      <c r="C100" s="45" t="s">
-        <v>757</v>
-      </c>
-      <c r="D100" s="45" t="s">
-        <v>757</v>
-      </c>
-      <c r="E100" s="45" t="s">
+      <c r="B100" s="44" t="s">
+        <v>711</v>
+      </c>
+      <c r="C100" s="44" t="s">
+        <v>710</v>
+      </c>
+      <c r="D100" s="44" t="s">
+        <v>710</v>
+      </c>
+      <c r="E100" s="44" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="101" spans="1:18" s="55" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B101" s="55" t="s">
-        <v>21</v>
-      </c>
-      <c r="D101" s="55" t="s">
-        <v>761</v>
-      </c>
-      <c r="E101" s="55" t="s">
-        <v>759</v>
-      </c>
-      <c r="F101" s="62"/>
-      <c r="G101" s="55" t="s">
+    <row r="101" spans="1:18" s="54" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B101" s="54" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="54" t="s">
+        <v>714</v>
+      </c>
+      <c r="E101" s="54" t="s">
+        <v>712</v>
+      </c>
+      <c r="F101" s="61"/>
+      <c r="G101" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="H101" s="55" t="s">
-        <v>651</v>
-      </c>
-      <c r="I101" s="55">
+      <c r="H101" s="54" t="s">
+        <v>642</v>
+      </c>
+      <c r="I101" s="54">
         <v>1</v>
       </c>
-      <c r="J101" s="58"/>
-      <c r="K101" s="57">
+      <c r="J101" s="57"/>
+      <c r="K101" s="56">
         <v>0.9</v>
       </c>
-      <c r="L101" s="57">
+      <c r="L101" s="56">
         <v>1</v>
       </c>
-      <c r="M101" s="57">
+      <c r="M101" s="56">
         <v>0.95</v>
       </c>
-      <c r="N101" s="57">
+      <c r="N101" s="56">
         <f>(L101-K101)/6</f>
         <v>1.6666666666666663E-2</v>
       </c>
-      <c r="O101" s="57">
+      <c r="O101" s="56">
         <v>0.1</v>
       </c>
-      <c r="R101" s="39" t="s">
-        <v>803</v>
-      </c>
-    </row>
-    <row r="102" spans="1:18" s="39" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="R101" s="38" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="102" spans="1:18" s="38" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B102" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D102" s="39" t="s">
-        <v>762</v>
-      </c>
-      <c r="E102" s="39" t="s">
-        <v>760</v>
-      </c>
-      <c r="F102" s="49"/>
-      <c r="G102" s="39" t="s">
+      <c r="D102" s="38" t="s">
+        <v>715</v>
+      </c>
+      <c r="E102" s="38" t="s">
+        <v>713</v>
+      </c>
+      <c r="F102" s="48"/>
+      <c r="G102" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="H102" s="39" t="s">
-        <v>651</v>
-      </c>
-      <c r="I102" s="39">
+      <c r="H102" s="38" t="s">
+        <v>642</v>
+      </c>
+      <c r="I102" s="38">
         <v>1450</v>
       </c>
-      <c r="J102" s="42"/>
-      <c r="K102" s="41">
-        <v>0</v>
-      </c>
-      <c r="L102" s="41">
+      <c r="J102" s="41"/>
+      <c r="K102" s="40">
+        <v>0</v>
+      </c>
+      <c r="L102" s="40">
         <v>3000</v>
       </c>
-      <c r="M102" s="41">
+      <c r="M102" s="40">
         <v>1450</v>
       </c>
-      <c r="N102" s="41">
+      <c r="N102" s="40">
         <f>(L102-K102)/6</f>
         <v>500</v>
       </c>
-      <c r="O102" s="41">
+      <c r="O102" s="40">
         <v>50</v>
       </c>
-      <c r="R102" s="39" t="s">
-        <v>803</v>
+      <c r="R102" s="38" t="s">
+        <v>754</v>
       </c>
     </row>
     <row r="103" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A103" s="36"/>
-      <c r="B103" s="36"/>
-      <c r="C103" s="36"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="36"/>
-      <c r="G103" s="36"/>
-      <c r="H103" s="37"/>
-      <c r="I103" s="37"/>
-      <c r="J103" s="36"/>
-      <c r="K103" s="36"/>
-      <c r="L103" s="36"/>
-      <c r="M103" s="36"/>
-      <c r="N103" s="36"/>
-      <c r="O103" s="36"/>
-      <c r="P103" s="36"/>
-      <c r="Q103" s="36"/>
-      <c r="R103" s="36"/>
+      <c r="A103" s="35"/>
+      <c r="B103" s="35"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="35"/>
+      <c r="E103" s="35"/>
+      <c r="F103" s="35"/>
+      <c r="G103" s="35"/>
+      <c r="H103" s="36"/>
+      <c r="I103" s="36"/>
+      <c r="J103" s="35"/>
+      <c r="K103" s="35"/>
+      <c r="L103" s="35"/>
+      <c r="M103" s="35"/>
+      <c r="N103" s="35"/>
+      <c r="O103" s="35"/>
+      <c r="P103" s="35"/>
+      <c r="Q103" s="35"/>
+      <c r="R103" s="35"/>
     </row>
     <row r="104" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F104" s="62"/>
+      <c r="F104" s="61"/>
       <c r="I104" s="30"/>
       <c r="J104" s="30"/>
     </row>
     <row r="105" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F105" s="46"/>
+      <c r="F105" s="45"/>
       <c r="I105" s="30"/>
       <c r="J105" s="30"/>
     </row>
     <row r="106" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F106" s="46"/>
+      <c r="F106" s="45"/>
       <c r="I106" s="30"/>
       <c r="J106" s="30"/>
     </row>
     <row r="107" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F107" s="46"/>
+      <c r="F107" s="45"/>
       <c r="I107" s="30"/>
       <c r="J107" s="30"/>
     </row>
     <row r="108" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F108" s="46"/>
+      <c r="F108" s="45"/>
       <c r="I108" s="30"/>
       <c r="J108" s="30"/>
     </row>
     <row r="109" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F109" s="46"/>
+      <c r="F109" s="45"/>
       <c r="I109" s="30"/>
       <c r="J109" s="30"/>
     </row>
     <row r="110" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F110" s="46"/>
+      <c r="F110" s="45"/>
       <c r="I110" s="30"/>
       <c r="J110" s="30"/>
     </row>
     <row r="111" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F111" s="46"/>
+      <c r="F111" s="45"/>
       <c r="I111" s="30"/>
       <c r="J111" s="30"/>
     </row>
     <row r="112" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="F112" s="46"/>
+      <c r="F112" s="45"/>
       <c r="I112" s="30"/>
       <c r="J112" s="30"/>
     </row>
@@ -10240,11 +10092,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10264,7 +10116,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.35">
       <c r="A1" s="5"/>
-      <c r="B1" s="59"/>
+      <c r="B1" s="58"/>
       <c r="C1" s="5"/>
       <c r="D1" s="5"/>
       <c r="E1" s="7" t="s">
@@ -10282,11 +10134,11 @@
       <c r="A2" s="8" t="s">
         <v>457</v>
       </c>
-      <c r="B2" s="64" t="s">
-        <v>766</v>
+      <c r="B2" s="63" t="s">
+        <v>719</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="D2" s="8" t="s">
         <v>458</v>
@@ -10320,11 +10172,11 @@
       <c r="A3" s="14" t="s">
         <v>619</v>
       </c>
-      <c r="B3" s="64" t="s">
-        <v>767</v>
+      <c r="B3" s="63" t="s">
+        <v>720</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>632</v>
+        <v>626</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>622</v>
@@ -10352,18 +10204,18 @@
         <v>621</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>633</v>
+        <v>627</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="29" t="s">
-        <v>634</v>
+        <v>628</v>
       </c>
       <c r="C4" s="29" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="E4" s="29" t="s">
         <v>464</v>
@@ -10386,16 +10238,15 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="29" t="s">
-        <v>635</v>
-      </c>
-      <c r="C5" s="29" t="s">
-        <v>629</v>
-      </c>
+        <v>633</v>
+      </c>
+      <c r="B5" s="45"/>
+      <c r="C5" s="29"/>
       <c r="D5" s="29" t="s">
-        <v>626</v>
+        <v>757</v>
       </c>
       <c r="E5" s="29" t="s">
-        <v>464</v>
+        <v>634</v>
       </c>
       <c r="F5" s="29" t="s">
         <v>62</v>
@@ -10416,19 +10267,15 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="29" t="s">
+        <v>635</v>
+      </c>
+      <c r="B6" s="45"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="29" t="s">
+        <v>758</v>
+      </c>
+      <c r="E6" s="29" t="s">
         <v>636</v>
-      </c>
-      <c r="B6" s="46" t="s">
-        <v>768</v>
-      </c>
-      <c r="C6" s="29" t="s">
-        <v>631</v>
-      </c>
-      <c r="D6" s="29" t="s">
-        <v>623</v>
-      </c>
-      <c r="E6" s="29" t="s">
-        <v>464</v>
       </c>
       <c r="F6" s="29" t="s">
         <v>62</v>
@@ -10442,27 +10289,24 @@
       <c r="I6" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="31"/>
+      <c r="J6" s="29"/>
       <c r="K6" s="29"/>
       <c r="L6" s="29"/>
+      <c r="M6" s="29"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="29" t="s">
-        <v>637</v>
-      </c>
-      <c r="B7" s="46" t="s">
-        <v>769</v>
-      </c>
-      <c r="C7" s="29" t="s">
-        <v>630</v>
-      </c>
+        <v>665</v>
+      </c>
+      <c r="B7" s="45"/>
+      <c r="C7" s="29"/>
       <c r="D7" s="29" t="s">
-        <v>624</v>
+        <v>759</v>
       </c>
       <c r="E7" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F7" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F7" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G7" s="29" t="b">
@@ -10474,23 +10318,23 @@
       <c r="I7" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J7" s="31"/>
       <c r="K7" s="29"/>
       <c r="L7" s="29"/>
+      <c r="M7" s="29"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="29" t="s">
-        <v>674</v>
-      </c>
-      <c r="B8" s="46"/>
+        <v>666</v>
+      </c>
+      <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>675</v>
+        <v>760</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F8" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F8" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G8" s="29" t="b">
@@ -10502,63 +10346,61 @@
       <c r="I8" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J8" s="29"/>
       <c r="K8" s="29"/>
       <c r="L8" s="29"/>
       <c r="M8" s="29"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="29" t="s">
-        <v>676</v>
-      </c>
-      <c r="B9" s="46"/>
+        <v>667</v>
+      </c>
+      <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>677</v>
+        <v>761</v>
       </c>
       <c r="E9" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F9" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F9" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G9" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I9" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J9" s="29"/>
+        <v>1</v>
+      </c>
       <c r="K9" s="29"/>
       <c r="L9" s="29"/>
       <c r="M9" s="29"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="29" t="s">
-        <v>678</v>
-      </c>
-      <c r="B10" s="46"/>
+        <v>668</v>
+      </c>
+      <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29" t="s">
-        <v>679</v>
+        <v>762</v>
       </c>
       <c r="E10" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F10" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F10" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G10" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I10" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="29"/>
       <c r="L10" s="29"/>
@@ -10566,27 +10408,27 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" s="29" t="s">
-        <v>680</v>
-      </c>
-      <c r="B11" s="46"/>
+        <v>669</v>
+      </c>
+      <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>681</v>
+        <v>763</v>
       </c>
       <c r="E11" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F11" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F11" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G11" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I11" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" s="29"/>
       <c r="L11" s="29"/>
@@ -10594,27 +10436,27 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="29" t="s">
-        <v>682</v>
-      </c>
-      <c r="B12" s="46"/>
+        <v>670</v>
+      </c>
+      <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>683</v>
+        <v>764</v>
       </c>
       <c r="E12" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F12" s="29" t="s">
+        <v>642</v>
+      </c>
+      <c r="F12" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G12" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" s="29" t="b">
         <v>1</v>
       </c>
       <c r="I12" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K12" s="29"/>
       <c r="L12" s="29"/>
@@ -10622,21 +10464,19 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="29" t="s">
-        <v>684</v>
-      </c>
-      <c r="B13" s="46"/>
+        <v>692</v>
+      </c>
+      <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>685</v>
-      </c>
-      <c r="E13" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F13" s="29" t="s">
+        <v>765</v>
+      </c>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G13" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" s="29" t="b">
         <v>1</v>
@@ -10644,27 +10484,22 @@
       <c r="I13" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="K13" s="29"/>
-      <c r="L13" s="29"/>
-      <c r="M13" s="29"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="29" t="s">
-        <v>686</v>
-      </c>
-      <c r="B14" s="46"/>
+        <v>693</v>
+      </c>
+      <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>687</v>
-      </c>
-      <c r="E14" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F14" s="29" t="s">
+        <v>766</v>
+      </c>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G14" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" s="29" t="b">
         <v>1</v>
@@ -10672,28 +10507,22 @@
       <c r="I14" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J14" s="29"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="29"/>
-      <c r="M14" s="29"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="29" t="s">
-        <v>688</v>
-      </c>
-      <c r="B15" s="46"/>
+        <v>694</v>
+      </c>
+      <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="29" t="s">
-        <v>689</v>
-      </c>
-      <c r="E15" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F15" s="29" t="s">
+        <v>767</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G15" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="29" t="b">
         <v>1</v>
@@ -10701,28 +10530,20 @@
       <c r="I15" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J15" s="29"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="29" t="s">
-        <v>690</v>
-      </c>
-      <c r="B16" s="46"/>
-      <c r="C16" s="29"/>
+        <v>695</v>
+      </c>
+      <c r="B16" s="29"/>
       <c r="D16" s="29" t="s">
-        <v>691</v>
-      </c>
-      <c r="E16" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F16" s="29" t="s">
+        <v>768</v>
+      </c>
+      <c r="F16" s="30" t="s">
         <v>62</v>
       </c>
       <c r="G16" s="29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" s="29" t="b">
         <v>1</v>
@@ -10730,619 +10551,101 @@
       <c r="I16" s="29" t="b">
         <v>0</v>
       </c>
-      <c r="J16" s="29"/>
-      <c r="K16" s="29"/>
-      <c r="L16" s="29"/>
-      <c r="M16" s="29"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="29" t="s">
-        <v>692</v>
-      </c>
-      <c r="B17" s="46"/>
-      <c r="C17" s="29"/>
-      <c r="D17" s="29" t="s">
-        <v>693</v>
-      </c>
-      <c r="E17" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F17" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H17" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I17" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J17" s="29"/>
-      <c r="K17" s="29"/>
-      <c r="L17" s="29"/>
-      <c r="M17" s="29"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="29" t="s">
-        <v>694</v>
-      </c>
-      <c r="B18" s="46"/>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29" t="s">
-        <v>695</v>
-      </c>
-      <c r="E18" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F18" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H18" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I18" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J18" s="29"/>
-      <c r="K18" s="29"/>
-      <c r="L18" s="29"/>
-      <c r="M18" s="29"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A19" s="29" t="s">
-        <v>696</v>
-      </c>
-      <c r="B19" s="46"/>
-      <c r="C19" s="29"/>
-      <c r="D19" s="29" t="s">
-        <v>697</v>
-      </c>
-      <c r="E19" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F19" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G19" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H19" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I19" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J19" s="29"/>
-      <c r="K19" s="29"/>
-      <c r="L19" s="29"/>
-      <c r="M19" s="29"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="29" t="s">
-        <v>698</v>
-      </c>
-      <c r="B20" s="46"/>
-      <c r="C20" s="29"/>
-      <c r="D20" s="29" t="s">
-        <v>699</v>
-      </c>
-      <c r="E20" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F20" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G20" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I20" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J20" s="29"/>
-      <c r="K20" s="29"/>
-      <c r="L20" s="29"/>
-      <c r="M20" s="29"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A21" s="29" t="s">
-        <v>700</v>
-      </c>
-      <c r="B21" s="46"/>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29" t="s">
-        <v>701</v>
-      </c>
-      <c r="E21" s="29" t="s">
-        <v>464</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G21" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H21" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I21" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J21" s="29"/>
-      <c r="K21" s="29"/>
-      <c r="L21" s="29"/>
-      <c r="M21" s="29"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A22" s="29" t="s">
-        <v>702</v>
-      </c>
-      <c r="B22" s="46"/>
-      <c r="C22" s="29"/>
-      <c r="D22" s="29" t="s">
-        <v>703</v>
-      </c>
-      <c r="E22" s="29" t="s">
-        <v>704</v>
-      </c>
-      <c r="F22" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G22" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H22" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I22" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J22" s="29"/>
-      <c r="K22" s="29"/>
-      <c r="L22" s="29"/>
-      <c r="M22" s="29"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="29" t="s">
-        <v>705</v>
-      </c>
-      <c r="B23" s="46"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29" t="s">
-        <v>706</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>704</v>
-      </c>
-      <c r="F23" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G23" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I23" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J23" s="29"/>
-      <c r="K23" s="29"/>
-      <c r="L23" s="29"/>
-      <c r="M23" s="29"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="29" t="s">
-        <v>707</v>
-      </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29" t="s">
-        <v>708</v>
-      </c>
-      <c r="E24" s="29" t="s">
-        <v>704</v>
-      </c>
-      <c r="F24" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G24" s="46" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I24" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J24" s="29"/>
-      <c r="K24" s="29"/>
-      <c r="L24" s="29"/>
-      <c r="M24" s="29"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="29" t="s">
-        <v>709</v>
-      </c>
-      <c r="B25" s="46"/>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29" t="s">
-        <v>710</v>
-      </c>
-      <c r="E25" s="29" t="s">
-        <v>711</v>
-      </c>
-      <c r="F25" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G25" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I25" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J25" s="29"/>
-      <c r="K25" s="29"/>
-      <c r="L25" s="29"/>
-      <c r="M25" s="29"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
-        <v>642</v>
-      </c>
-      <c r="B26" s="46"/>
-      <c r="C26" s="29"/>
-      <c r="D26" s="29" t="s">
-        <v>806</v>
-      </c>
-      <c r="E26" s="29" t="s">
-        <v>643</v>
-      </c>
-      <c r="F26" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G26" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H26" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I26" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J26" s="29"/>
-      <c r="K26" s="29"/>
-      <c r="L26" s="29"/>
-      <c r="M26" s="29"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="29" t="s">
-        <v>644</v>
-      </c>
-      <c r="B27" s="46"/>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29" t="s">
-        <v>807</v>
-      </c>
-      <c r="E27" s="29" t="s">
-        <v>645</v>
-      </c>
-      <c r="F27" s="29" t="s">
-        <v>62</v>
-      </c>
-      <c r="G27" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H27" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I27" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="J27" s="29"/>
-      <c r="K27" s="29"/>
-      <c r="L27" s="29"/>
-      <c r="M27" s="29"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="29" t="s">
-        <v>712</v>
-      </c>
-      <c r="B28" s="46"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29" t="s">
-        <v>808</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F28" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G28" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H28" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I28" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K28" s="29"/>
-      <c r="L28" s="29"/>
-      <c r="M28" s="29"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="29" t="s">
-        <v>713</v>
-      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B17" s="29"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B18" s="29"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B19" s="29"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B20" s="29"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21" s="29"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B22" s="29"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B23" s="29"/>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B24" s="29"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B25" s="29"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B26" s="29"/>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B27" s="29"/>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B28" s="29"/>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29" t="s">
-        <v>809</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G29" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="H29" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I29" s="29" t="b">
-        <v>0</v>
-      </c>
-      <c r="K29" s="29"/>
-      <c r="L29" s="29"/>
-      <c r="M29" s="29"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="29" t="s">
-        <v>714</v>
-      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29" t="s">
-        <v>810</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F30" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G30" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I30" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K30" s="29"/>
-      <c r="L30" s="29"/>
-      <c r="M30" s="29"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="29" t="s">
-        <v>715</v>
-      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29" t="s">
-        <v>811</v>
-      </c>
-      <c r="E31" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F31" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G31" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I31" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K31" s="29"/>
-      <c r="L31" s="29"/>
-      <c r="M31" s="29"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A32" s="29" t="s">
-        <v>716</v>
-      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29" t="s">
-        <v>812</v>
-      </c>
-      <c r="E32" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G32" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I32" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K32" s="29"/>
-      <c r="L32" s="29"/>
-      <c r="M32" s="29"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A33" s="29" t="s">
-        <v>717</v>
-      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29" t="s">
-        <v>813</v>
-      </c>
-      <c r="E33" s="29" t="s">
-        <v>651</v>
-      </c>
-      <c r="F33" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G33" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I33" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="K33" s="29"/>
-      <c r="L33" s="29"/>
-      <c r="M33" s="29"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A34" s="29" t="s">
-        <v>739</v>
-      </c>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B34" s="29"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29" t="s">
-        <v>814</v>
-      </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G34" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I34" s="29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A35" s="29" t="s">
-        <v>740</v>
-      </c>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29" t="s">
-        <v>815</v>
-      </c>
-      <c r="E35" s="29"/>
-      <c r="F35" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G35" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I35" s="29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A36" s="29" t="s">
-        <v>741</v>
-      </c>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B36" s="29"/>
-      <c r="C36" s="29"/>
-      <c r="D36" s="29" t="s">
-        <v>816</v>
-      </c>
-      <c r="E36" s="29"/>
-      <c r="F36" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G36" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I36" s="29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A37" s="29" t="s">
-        <v>742</v>
-      </c>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B37" s="29"/>
-      <c r="D37" s="29" t="s">
-        <v>817</v>
-      </c>
-      <c r="F37" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G37" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="29" t="b">
-        <v>1</v>
-      </c>
-      <c r="I37" s="29" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B38" s="29"/>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B39" s="29"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B40" s="29"/>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B41" s="29"/>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B42" s="29"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B43" s="29"/>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B44" s="29"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B45" s="29"/>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B46" s="29"/>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B47" s="29"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B48" s="29"/>
     </row>
     <row r="49" spans="2:2" x14ac:dyDescent="0.3">
@@ -11419,69 +10722,6 @@
     </row>
     <row r="73" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B73" s="29"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B74" s="29"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B75" s="29"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B76" s="29"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B77" s="29"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B78" s="29"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B79" s="29"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B80" s="29"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B81" s="29"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B82" s="29"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B83" s="29"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B84" s="29"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B85" s="29"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B86" s="29"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B87" s="29"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B88" s="29"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B89" s="29"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B90" s="29"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B91" s="29"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B92" s="29"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B93" s="29"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B94" s="29"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -20100,7 +19340,7 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>639</v>
+        <v>630</v>
       </c>
       <c r="L24" s="1" t="s">
         <v>553</v>

</xml_diff>

<commit_message>
how did this get deleted?
</commit_message>
<xml_diff>
--- a/projects/SEB_calibration_NSGA_2013.xlsx
+++ b/projects/SEB_calibration_NSGA_2013.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562"/>
+    <workbookView xWindow="10188" yWindow="-216" windowWidth="23256" windowHeight="13176" tabRatio="562" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Setup" sheetId="7" r:id="rId1"/>
@@ -2313,40 +2313,40 @@
     <t>CalibrationReportsEnhanced20</t>
   </si>
   <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_consumption_modeled</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_rmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_consumption_cvrmse</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_consumption_nmbe</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.electricity_nmbe_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_cvrmse_within_limit</t>
-  </si>
-  <si>
-    <t>calibration_reports_enhanced20.gas_nmbe_within_limit</t>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_modeled</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_rmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.electricity_nmbe_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_modeled</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_rmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_cvrmse</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_consumption_nmbe</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_cvrmse_within_limit</t>
+  </si>
+  <si>
+    <t>CalibrationReportsEnhanced20.natural_gas_nmbe_within_limit</t>
   </si>
 </sst>
 </file>
@@ -6641,7 +6641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -10094,9 +10094,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M73"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10272,7 +10272,7 @@
       <c r="B6" s="45"/>
       <c r="C6" s="29"/>
       <c r="D6" s="29" t="s">
-        <v>758</v>
+        <v>763</v>
       </c>
       <c r="E6" s="29" t="s">
         <v>636</v>
@@ -10301,7 +10301,7 @@
       <c r="B7" s="45"/>
       <c r="C7" s="29"/>
       <c r="D7" s="29" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="E7" s="29" t="s">
         <v>642</v>
@@ -10329,7 +10329,7 @@
       <c r="B8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="29" t="s">
-        <v>760</v>
+        <v>764</v>
       </c>
       <c r="E8" s="29" t="s">
         <v>642</v>
@@ -10357,7 +10357,7 @@
       <c r="B9" s="29"/>
       <c r="C9" s="29"/>
       <c r="D9" s="29" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="E9" s="29" t="s">
         <v>642</v>
@@ -10385,7 +10385,7 @@
       <c r="B10" s="29"/>
       <c r="C10" s="29"/>
       <c r="D10" s="29" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="E10" s="29" t="s">
         <v>642</v>
@@ -10413,7 +10413,7 @@
       <c r="B11" s="29"/>
       <c r="C11" s="29"/>
       <c r="D11" s="29" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>642</v>
@@ -10441,7 +10441,7 @@
       <c r="B12" s="29"/>
       <c r="C12" s="29"/>
       <c r="D12" s="29" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>642</v>
@@ -10469,7 +10469,7 @@
       <c r="B13" s="29"/>
       <c r="C13" s="29"/>
       <c r="D13" s="29" t="s">
-        <v>765</v>
+        <v>761</v>
       </c>
       <c r="E13" s="29"/>
       <c r="F13" s="30" t="s">
@@ -10492,7 +10492,7 @@
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="29" t="s">
-        <v>766</v>
+        <v>762</v>
       </c>
       <c r="E14" s="29"/>
       <c r="F14" s="30" t="s">

</xml_diff>